<commit_message>
added admob and changed database
</commit_message>
<xml_diff>
--- a/app/src/main/assets/Korean Phrases-Ko_secondDraft_Romanization_Done v2.xlsx
+++ b/app/src/main/assets/Korean Phrases-Ko_secondDraft_Romanization_Done v2.xlsx
@@ -1443,7 +1443,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6696" uniqueCount="2737">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6696" uniqueCount="2739">
   <si>
     <t>Basics</t>
   </si>
@@ -11416,6 +11416,12 @@
   </si>
   <si>
     <t>eonje mun dadeusinayo?</t>
+  </si>
+  <si>
+    <t>Travel</t>
+  </si>
+  <si>
+    <t>Taxi</t>
   </si>
 </sst>
 </file>
@@ -11548,28 +11554,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -11857,7 +11842,7 @@
     <col min="1" max="1" width="43.44140625" customWidth="1"/>
     <col min="2" max="2" width="36.88671875" style="4" customWidth="1"/>
     <col min="3" max="3" width="33.109375" customWidth="1"/>
-    <col min="4" max="4" width="50.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="106" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -23664,7 +23649,7 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67">
-        <f t="shared" ref="A67:A129" si="1">A66+1</f>
+        <f t="shared" ref="A67:A130" si="1">A66+1</f>
         <v>67</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -24987,7 +24972,7 @@
     </row>
     <row r="130" spans="1:6">
       <c r="A130">
-        <f t="shared" ref="A130:A193" si="2">A129+1</f>
+        <f t="shared" si="1"/>
         <v>130</v>
       </c>
       <c r="B130" s="4" t="s">
@@ -25008,7 +24993,7 @@
     </row>
     <row r="131" spans="1:6">
       <c r="A131">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="A131:A194" si="2">A130+1</f>
         <v>131</v>
       </c>
       <c r="B131" s="4" t="s">
@@ -26331,7 +26316,7 @@
     </row>
     <row r="194" spans="1:6">
       <c r="A194">
-        <f t="shared" ref="A194:A257" si="3">A193+1</f>
+        <f t="shared" si="2"/>
         <v>194</v>
       </c>
       <c r="B194" s="4" t="s">
@@ -26352,7 +26337,7 @@
     </row>
     <row r="195" spans="1:6">
       <c r="A195">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="A195:A258" si="3">A194+1</f>
         <v>195</v>
       </c>
       <c r="B195" s="4" t="s">
@@ -26818,7 +26803,7 @@
         <v>217</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>473</v>
@@ -26839,7 +26824,7 @@
         <v>218</v>
       </c>
       <c r="B218" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C218" s="4" t="s">
         <v>474</v>
@@ -26860,7 +26845,7 @@
         <v>219</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C219" s="4" t="s">
         <v>475</v>
@@ -26881,7 +26866,7 @@
         <v>220</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C220" s="4" t="s">
         <v>476</v>
@@ -26902,7 +26887,7 @@
         <v>221</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C221" s="4" t="s">
         <v>477</v>
@@ -26923,7 +26908,7 @@
         <v>222</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C222" s="4" t="s">
         <v>478</v>
@@ -26944,7 +26929,7 @@
         <v>223</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C223" s="4" t="s">
         <v>479</v>
@@ -26965,7 +26950,7 @@
         <v>224</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>480</v>
@@ -26986,7 +26971,7 @@
         <v>225</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C225" s="4" t="s">
         <v>481</v>
@@ -27007,7 +26992,7 @@
         <v>226</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C226" s="4" t="s">
         <v>482</v>
@@ -27028,7 +27013,7 @@
         <v>227</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C227" s="4" t="s">
         <v>483</v>
@@ -27049,7 +27034,7 @@
         <v>228</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C228" s="4" t="s">
         <v>484</v>
@@ -27070,7 +27055,7 @@
         <v>229</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C229" s="4" t="s">
         <v>485</v>
@@ -27091,7 +27076,7 @@
         <v>230</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>486</v>
@@ -27112,7 +27097,7 @@
         <v>231</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C231" s="4" t="s">
         <v>44</v>
@@ -27133,7 +27118,7 @@
         <v>232</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C232" s="4" t="s">
         <v>487</v>
@@ -27154,7 +27139,7 @@
         <v>233</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>488</v>
@@ -27175,7 +27160,7 @@
         <v>234</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C234" s="4" t="s">
         <v>489</v>
@@ -27196,7 +27181,7 @@
         <v>235</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C235" s="4" t="s">
         <v>490</v>
@@ -27217,7 +27202,7 @@
         <v>236</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C236" s="4" t="s">
         <v>491</v>
@@ -27238,7 +27223,7 @@
         <v>237</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C237" s="4" t="s">
         <v>492</v>
@@ -27259,7 +27244,7 @@
         <v>238</v>
       </c>
       <c r="B238" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C238" s="4" t="s">
         <v>493</v>
@@ -27280,7 +27265,7 @@
         <v>239</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C239" s="4" t="s">
         <v>494</v>
@@ -27301,7 +27286,7 @@
         <v>240</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C240" s="4" t="s">
         <v>495</v>
@@ -27322,7 +27307,7 @@
         <v>241</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C241" s="4" t="s">
         <v>496</v>
@@ -27343,7 +27328,7 @@
         <v>242</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C242" s="4" t="s">
         <v>497</v>
@@ -27364,7 +27349,7 @@
         <v>243</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C243" s="4" t="s">
         <v>498</v>
@@ -27385,7 +27370,7 @@
         <v>244</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C244" s="4" t="s">
         <v>499</v>
@@ -27406,7 +27391,7 @@
         <v>245</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C245" s="4" t="s">
         <v>500</v>
@@ -27427,7 +27412,7 @@
         <v>246</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C246" s="4" t="s">
         <v>501</v>
@@ -27448,7 +27433,7 @@
         <v>247</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C247" s="4" t="s">
         <v>502</v>
@@ -27469,7 +27454,7 @@
         <v>248</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C248" s="4" t="s">
         <v>503</v>
@@ -27490,7 +27475,7 @@
         <v>249</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C249" s="4" t="s">
         <v>504</v>
@@ -27511,7 +27496,7 @@
         <v>250</v>
       </c>
       <c r="B250" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C250" s="4" t="s">
         <v>505</v>
@@ -27532,7 +27517,7 @@
         <v>251</v>
       </c>
       <c r="B251" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C251" s="4" t="s">
         <v>506</v>
@@ -27553,7 +27538,7 @@
         <v>252</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C252" s="4" t="s">
         <v>507</v>
@@ -27574,7 +27559,7 @@
         <v>253</v>
       </c>
       <c r="B253" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C253" s="4" t="s">
         <v>508</v>
@@ -27595,7 +27580,7 @@
         <v>254</v>
       </c>
       <c r="B254" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C254" s="4" t="s">
         <v>509</v>
@@ -27616,7 +27601,7 @@
         <v>255</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C255" s="4" t="s">
         <v>510</v>
@@ -27637,7 +27622,7 @@
         <v>256</v>
       </c>
       <c r="B256" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C256" s="4" t="s">
         <v>511</v>
@@ -27658,7 +27643,7 @@
         <v>257</v>
       </c>
       <c r="B257" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C257" s="4" t="s">
         <v>512</v>
@@ -27675,11 +27660,11 @@
     </row>
     <row r="258" spans="1:6">
       <c r="A258">
-        <f t="shared" ref="A258:A320" si="4">A257+1</f>
+        <f t="shared" si="3"/>
         <v>258</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>472</v>
+        <v>2737</v>
       </c>
       <c r="C258" s="4" t="s">
         <v>513</v>
@@ -27696,11 +27681,11 @@
     </row>
     <row r="259" spans="1:6">
       <c r="A259">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="A259:A322" si="4">A258+1</f>
         <v>259</v>
       </c>
       <c r="B259" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C259" s="4" t="s">
         <v>625</v>
@@ -27721,7 +27706,7 @@
         <v>260</v>
       </c>
       <c r="B260" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C260" s="4" t="s">
         <v>626</v>
@@ -27742,7 +27727,7 @@
         <v>261</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C261" s="4" t="s">
         <v>627</v>
@@ -27763,7 +27748,7 @@
         <v>262</v>
       </c>
       <c r="B262" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C262" s="4" t="s">
         <v>628</v>
@@ -27784,7 +27769,7 @@
         <v>263</v>
       </c>
       <c r="B263" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C263" s="4" t="s">
         <v>629</v>
@@ -27805,7 +27790,7 @@
         <v>264</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C264" s="4" t="s">
         <v>630</v>
@@ -27826,7 +27811,7 @@
         <v>265</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C265" s="4" t="s">
         <v>631</v>
@@ -27847,7 +27832,7 @@
         <v>266</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C266" s="4" t="s">
         <v>632</v>
@@ -27868,7 +27853,7 @@
         <v>267</v>
       </c>
       <c r="B267" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C267" s="4" t="s">
         <v>633</v>
@@ -27889,7 +27874,7 @@
         <v>268</v>
       </c>
       <c r="B268" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C268" s="4" t="s">
         <v>634</v>
@@ -27910,7 +27895,7 @@
         <v>269</v>
       </c>
       <c r="B269" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C269" s="4" t="s">
         <v>635</v>
@@ -27931,7 +27916,7 @@
         <v>270</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C270" s="4" t="s">
         <v>636</v>
@@ -27952,7 +27937,7 @@
         <v>271</v>
       </c>
       <c r="B271" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C271" s="4" t="s">
         <v>637</v>
@@ -27973,7 +27958,7 @@
         <v>272</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C272" s="4" t="s">
         <v>639</v>
@@ -27994,7 +27979,7 @@
         <v>273</v>
       </c>
       <c r="B273" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C273" s="4" t="s">
         <v>640</v>
@@ -28015,7 +28000,7 @@
         <v>274</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C274" s="4" t="s">
         <v>641</v>
@@ -28036,7 +28021,7 @@
         <v>275</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C275" s="4" t="s">
         <v>642</v>
@@ -28057,7 +28042,7 @@
         <v>276</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C276" s="4" t="s">
         <v>643</v>
@@ -28078,7 +28063,7 @@
         <v>277</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C277" s="4" t="s">
         <v>644</v>
@@ -28099,7 +28084,7 @@
         <v>278</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C278" s="4" t="s">
         <v>645</v>
@@ -28120,7 +28105,7 @@
         <v>279</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C279" s="4" t="s">
         <v>646</v>
@@ -28141,7 +28126,7 @@
         <v>280</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>604</v>
+        <v>2738</v>
       </c>
       <c r="C280" s="4" t="s">
         <v>647</v>
@@ -28998,7 +28983,7 @@
     </row>
     <row r="321" spans="1:6">
       <c r="A321">
-        <f t="shared" ref="A321:A383" si="5">A320+1</f>
+        <f t="shared" si="4"/>
         <v>321</v>
       </c>
       <c r="B321" s="4" t="s">
@@ -29019,7 +29004,7 @@
     </row>
     <row r="322" spans="1:6">
       <c r="A322">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>322</v>
       </c>
       <c r="B322" s="4" t="s">
@@ -29040,7 +29025,7 @@
     </row>
     <row r="323" spans="1:6">
       <c r="A323">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="A323:A386" si="5">A322+1</f>
         <v>323</v>
       </c>
       <c r="B323" s="4" t="s">
@@ -30321,7 +30306,7 @@
     </row>
     <row r="384" spans="1:6">
       <c r="A384">
-        <f t="shared" ref="A384:A446" si="6">A383+1</f>
+        <f t="shared" si="5"/>
         <v>384</v>
       </c>
       <c r="B384" s="4" t="s">
@@ -30342,7 +30327,7 @@
     </row>
     <row r="385" spans="1:6">
       <c r="A385">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>385</v>
       </c>
       <c r="B385" s="4" t="s">
@@ -30363,7 +30348,7 @@
     </row>
     <row r="386" spans="1:6">
       <c r="A386">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>386</v>
       </c>
       <c r="B386" s="4" t="s">
@@ -30384,7 +30369,7 @@
     </row>
     <row r="387" spans="1:6">
       <c r="A387">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="A387:A450" si="6">A386+1</f>
         <v>387</v>
       </c>
       <c r="B387" s="4" t="s">
@@ -31644,7 +31629,7 @@
     </row>
     <row r="447" spans="1:6">
       <c r="A447">
-        <f t="shared" ref="A447:A510" si="7">A446+1</f>
+        <f t="shared" si="6"/>
         <v>447</v>
       </c>
       <c r="B447" s="4" t="s">
@@ -31665,7 +31650,7 @@
     </row>
     <row r="448" spans="1:6">
       <c r="A448">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>448</v>
       </c>
       <c r="B448" s="4" t="s">
@@ -31686,7 +31671,7 @@
     </row>
     <row r="449" spans="1:6">
       <c r="A449">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>449</v>
       </c>
       <c r="B449" s="4" t="s">
@@ -31707,7 +31692,7 @@
     </row>
     <row r="450" spans="1:6">
       <c r="A450">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>450</v>
       </c>
       <c r="B450" s="4" t="s">
@@ -31728,7 +31713,7 @@
     </row>
     <row r="451" spans="1:6">
       <c r="A451">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="A451:A514" si="7">A450+1</f>
         <v>451</v>
       </c>
       <c r="B451" s="4" t="s">
@@ -32988,7 +32973,7 @@
     </row>
     <row r="511" spans="1:6">
       <c r="A511">
-        <f t="shared" ref="A511:A556" si="8">A510+1</f>
+        <f t="shared" si="7"/>
         <v>511</v>
       </c>
       <c r="B511" s="4" t="s">
@@ -33009,7 +32994,7 @@
     </row>
     <row r="512" spans="1:6">
       <c r="A512">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>512</v>
       </c>
       <c r="B512" s="4" t="s">
@@ -33030,7 +33015,7 @@
     </row>
     <row r="513" spans="1:6">
       <c r="A513">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>513</v>
       </c>
       <c r="B513" s="4" t="s">
@@ -33051,7 +33036,7 @@
     </row>
     <row r="514" spans="1:6">
       <c r="A514">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>514</v>
       </c>
       <c r="B514" s="4" t="s">
@@ -33072,7 +33057,7 @@
     </row>
     <row r="515" spans="1:6">
       <c r="A515">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="A515:A578" si="8">A514+1</f>
         <v>515</v>
       </c>
       <c r="B515" s="4" t="s">
@@ -33954,7 +33939,7 @@
     </row>
     <row r="557" spans="1:6">
       <c r="A557">
-        <f t="shared" ref="A557:A620" si="9">A556+1</f>
+        <f t="shared" si="8"/>
         <v>557</v>
       </c>
       <c r="B557" s="4" t="s">
@@ -33975,7 +33960,7 @@
     </row>
     <row r="558" spans="1:6">
       <c r="A558">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>558</v>
       </c>
       <c r="B558" s="4" t="s">
@@ -33996,7 +33981,7 @@
     </row>
     <row r="559" spans="1:6">
       <c r="A559">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>559</v>
       </c>
       <c r="B559" s="4" t="s">
@@ -34017,7 +34002,7 @@
     </row>
     <row r="560" spans="1:6">
       <c r="A560">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>560</v>
       </c>
       <c r="B560" s="4" t="s">
@@ -34038,7 +34023,7 @@
     </row>
     <row r="561" spans="1:6">
       <c r="A561">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>561</v>
       </c>
       <c r="B561" s="4" t="s">
@@ -34059,7 +34044,7 @@
     </row>
     <row r="562" spans="1:6">
       <c r="A562">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>562</v>
       </c>
       <c r="B562" s="4" t="s">
@@ -34080,7 +34065,7 @@
     </row>
     <row r="563" spans="1:6">
       <c r="A563">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>563</v>
       </c>
       <c r="B563" s="4" t="s">
@@ -34101,7 +34086,7 @@
     </row>
     <row r="564" spans="1:6">
       <c r="A564">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>564</v>
       </c>
       <c r="B564" s="4" t="s">
@@ -34122,7 +34107,7 @@
     </row>
     <row r="565" spans="1:6">
       <c r="A565">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>565</v>
       </c>
       <c r="B565" s="4" t="s">
@@ -34143,7 +34128,7 @@
     </row>
     <row r="566" spans="1:6">
       <c r="A566">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>566</v>
       </c>
       <c r="B566" s="4" t="s">
@@ -34164,7 +34149,7 @@
     </row>
     <row r="567" spans="1:6">
       <c r="A567">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>567</v>
       </c>
       <c r="B567" s="4" t="s">
@@ -34185,7 +34170,7 @@
     </row>
     <row r="568" spans="1:6">
       <c r="A568">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>568</v>
       </c>
       <c r="B568" s="4" t="s">
@@ -34206,7 +34191,7 @@
     </row>
     <row r="569" spans="1:6">
       <c r="A569">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>569</v>
       </c>
       <c r="B569" s="4" t="s">
@@ -34227,7 +34212,7 @@
     </row>
     <row r="570" spans="1:6">
       <c r="A570">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>570</v>
       </c>
       <c r="B570" s="4" t="s">
@@ -34248,7 +34233,7 @@
     </row>
     <row r="571" spans="1:6">
       <c r="A571">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>571</v>
       </c>
       <c r="B571" s="4" t="s">
@@ -34269,7 +34254,7 @@
     </row>
     <row r="572" spans="1:6">
       <c r="A572">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>572</v>
       </c>
       <c r="B572" s="4" t="s">
@@ -34290,7 +34275,7 @@
     </row>
     <row r="573" spans="1:6">
       <c r="A573">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>573</v>
       </c>
       <c r="B573" s="4" t="s">
@@ -34311,7 +34296,7 @@
     </row>
     <row r="574" spans="1:6">
       <c r="A574">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>574</v>
       </c>
       <c r="B574" s="4" t="s">
@@ -34332,7 +34317,7 @@
     </row>
     <row r="575" spans="1:6">
       <c r="A575">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>575</v>
       </c>
       <c r="B575" s="4" t="s">
@@ -34353,7 +34338,7 @@
     </row>
     <row r="576" spans="1:6">
       <c r="A576">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>576</v>
       </c>
       <c r="B576" s="4" t="s">
@@ -34374,7 +34359,7 @@
     </row>
     <row r="577" spans="1:6">
       <c r="A577">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>577</v>
       </c>
       <c r="B577" s="4" t="s">
@@ -34395,7 +34380,7 @@
     </row>
     <row r="578" spans="1:6">
       <c r="A578">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>578</v>
       </c>
       <c r="B578" s="4" t="s">
@@ -34416,7 +34401,7 @@
     </row>
     <row r="579" spans="1:6">
       <c r="A579">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="A579:A642" si="9">A578+1</f>
         <v>579</v>
       </c>
       <c r="B579" s="4" t="s">
@@ -35298,7 +35283,7 @@
     </row>
     <row r="621" spans="1:6">
       <c r="A621">
-        <f t="shared" ref="A621:A684" si="10">A620+1</f>
+        <f t="shared" si="9"/>
         <v>621</v>
       </c>
       <c r="B621" s="4" t="s">
@@ -35319,7 +35304,7 @@
     </row>
     <row r="622" spans="1:6">
       <c r="A622">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>622</v>
       </c>
       <c r="B622" s="4" t="s">
@@ -35340,7 +35325,7 @@
     </row>
     <row r="623" spans="1:6">
       <c r="A623">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>623</v>
       </c>
       <c r="B623" s="4" t="s">
@@ -35361,7 +35346,7 @@
     </row>
     <row r="624" spans="1:6">
       <c r="A624">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>624</v>
       </c>
       <c r="B624" s="4" t="s">
@@ -35382,7 +35367,7 @@
     </row>
     <row r="625" spans="1:6">
       <c r="A625">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>625</v>
       </c>
       <c r="B625" s="4" t="s">
@@ -35403,7 +35388,7 @@
     </row>
     <row r="626" spans="1:6">
       <c r="A626">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>626</v>
       </c>
       <c r="B626" s="4" t="s">
@@ -35424,7 +35409,7 @@
     </row>
     <row r="627" spans="1:6">
       <c r="A627">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>627</v>
       </c>
       <c r="B627" s="4" t="s">
@@ -35445,7 +35430,7 @@
     </row>
     <row r="628" spans="1:6">
       <c r="A628">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>628</v>
       </c>
       <c r="B628" s="4" t="s">
@@ -35466,7 +35451,7 @@
     </row>
     <row r="629" spans="1:6">
       <c r="A629">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>629</v>
       </c>
       <c r="B629" s="4" t="s">
@@ -35487,7 +35472,7 @@
     </row>
     <row r="630" spans="1:6">
       <c r="A630">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>630</v>
       </c>
       <c r="B630" s="4" t="s">
@@ -35508,7 +35493,7 @@
     </row>
     <row r="631" spans="1:6">
       <c r="A631">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>631</v>
       </c>
       <c r="B631" s="4" t="s">
@@ -35529,7 +35514,7 @@
     </row>
     <row r="632" spans="1:6">
       <c r="A632">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>632</v>
       </c>
       <c r="B632" s="4" t="s">
@@ -35550,7 +35535,7 @@
     </row>
     <row r="633" spans="1:6">
       <c r="A633">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>633</v>
       </c>
       <c r="B633" s="4" t="s">
@@ -35571,7 +35556,7 @@
     </row>
     <row r="634" spans="1:6">
       <c r="A634">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>634</v>
       </c>
       <c r="B634" s="4" t="s">
@@ -35592,7 +35577,7 @@
     </row>
     <row r="635" spans="1:6">
       <c r="A635">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>635</v>
       </c>
       <c r="B635" s="4" t="s">
@@ -35613,7 +35598,7 @@
     </row>
     <row r="636" spans="1:6">
       <c r="A636">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>636</v>
       </c>
       <c r="B636" s="4" t="s">
@@ -35634,7 +35619,7 @@
     </row>
     <row r="637" spans="1:6">
       <c r="A637">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>637</v>
       </c>
       <c r="B637" s="4" t="s">
@@ -35655,7 +35640,7 @@
     </row>
     <row r="638" spans="1:6">
       <c r="A638">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>638</v>
       </c>
       <c r="B638" s="4" t="s">
@@ -35676,7 +35661,7 @@
     </row>
     <row r="639" spans="1:6">
       <c r="A639">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>639</v>
       </c>
       <c r="B639" s="4" t="s">
@@ -35697,7 +35682,7 @@
     </row>
     <row r="640" spans="1:6">
       <c r="A640">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>640</v>
       </c>
       <c r="B640" s="4" t="s">
@@ -35718,7 +35703,7 @@
     </row>
     <row r="641" spans="1:6">
       <c r="A641">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>641</v>
       </c>
       <c r="B641" s="4" t="s">
@@ -35739,7 +35724,7 @@
     </row>
     <row r="642" spans="1:6">
       <c r="A642">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>642</v>
       </c>
       <c r="B642" s="4" t="s">
@@ -35760,7 +35745,7 @@
     </row>
     <row r="643" spans="1:6">
       <c r="A643">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="A643:A706" si="10">A642+1</f>
         <v>643</v>
       </c>
       <c r="B643" s="4" t="s">
@@ -36642,7 +36627,7 @@
     </row>
     <row r="685" spans="1:6">
       <c r="A685">
-        <f t="shared" ref="A685:A744" si="11">A684+1</f>
+        <f t="shared" si="10"/>
         <v>685</v>
       </c>
       <c r="B685" s="4" t="s">
@@ -36663,7 +36648,7 @@
     </row>
     <row r="686" spans="1:6">
       <c r="A686">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>686</v>
       </c>
       <c r="B686" s="4" t="s">
@@ -36684,7 +36669,7 @@
     </row>
     <row r="687" spans="1:6">
       <c r="A687">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>687</v>
       </c>
       <c r="B687" s="4" t="s">
@@ -36705,7 +36690,7 @@
     </row>
     <row r="688" spans="1:6">
       <c r="A688">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>688</v>
       </c>
       <c r="B688" s="4" t="s">
@@ -36726,7 +36711,7 @@
     </row>
     <row r="689" spans="1:6">
       <c r="A689">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>689</v>
       </c>
       <c r="B689" s="4" t="s">
@@ -36747,7 +36732,7 @@
     </row>
     <row r="690" spans="1:6">
       <c r="A690">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>690</v>
       </c>
       <c r="B690" s="4" t="s">
@@ -36768,7 +36753,7 @@
     </row>
     <row r="691" spans="1:6">
       <c r="A691">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>691</v>
       </c>
       <c r="B691" s="4" t="s">
@@ -36789,7 +36774,7 @@
     </row>
     <row r="692" spans="1:6">
       <c r="A692">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>692</v>
       </c>
       <c r="B692" s="4" t="s">
@@ -36810,7 +36795,7 @@
     </row>
     <row r="693" spans="1:6">
       <c r="A693">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>693</v>
       </c>
       <c r="B693" s="4" t="s">
@@ -36831,7 +36816,7 @@
     </row>
     <row r="694" spans="1:6">
       <c r="A694">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>694</v>
       </c>
       <c r="B694" s="4" t="s">
@@ -36852,7 +36837,7 @@
     </row>
     <row r="695" spans="1:6">
       <c r="A695">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>695</v>
       </c>
       <c r="B695" s="4" t="s">
@@ -36873,7 +36858,7 @@
     </row>
     <row r="696" spans="1:6">
       <c r="A696">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>696</v>
       </c>
       <c r="B696" s="4" t="s">
@@ -36894,7 +36879,7 @@
     </row>
     <row r="697" spans="1:6">
       <c r="A697">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>697</v>
       </c>
       <c r="B697" s="4" t="s">
@@ -36915,7 +36900,7 @@
     </row>
     <row r="698" spans="1:6">
       <c r="A698">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>698</v>
       </c>
       <c r="B698" s="4" t="s">
@@ -36936,7 +36921,7 @@
     </row>
     <row r="699" spans="1:6">
       <c r="A699">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>699</v>
       </c>
       <c r="B699" s="4" t="s">
@@ -36957,7 +36942,7 @@
     </row>
     <row r="700" spans="1:6">
       <c r="A700">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>700</v>
       </c>
       <c r="B700" s="4" t="s">
@@ -36978,7 +36963,7 @@
     </row>
     <row r="701" spans="1:6">
       <c r="A701">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>701</v>
       </c>
       <c r="B701" s="4" t="s">
@@ -36999,7 +36984,7 @@
     </row>
     <row r="702" spans="1:6">
       <c r="A702">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>702</v>
       </c>
       <c r="B702" s="4" t="s">
@@ -37020,7 +37005,7 @@
     </row>
     <row r="703" spans="1:6">
       <c r="A703">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>703</v>
       </c>
       <c r="B703" s="4" t="s">
@@ -37041,7 +37026,7 @@
     </row>
     <row r="704" spans="1:6">
       <c r="A704">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>704</v>
       </c>
       <c r="B704" s="4" t="s">
@@ -37062,7 +37047,7 @@
     </row>
     <row r="705" spans="1:6">
       <c r="A705">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>705</v>
       </c>
       <c r="B705" s="4" t="s">
@@ -37083,7 +37068,7 @@
     </row>
     <row r="706" spans="1:6">
       <c r="A706">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>706</v>
       </c>
       <c r="B706" s="4" t="s">
@@ -37104,7 +37089,7 @@
     </row>
     <row r="707" spans="1:6">
       <c r="A707">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="A707:A770" si="11">A706+1</f>
         <v>707</v>
       </c>
       <c r="B707" s="4" t="s">
@@ -37902,7 +37887,7 @@
     </row>
     <row r="745" spans="1:6">
       <c r="A745">
-        <f t="shared" ref="A745:A803" si="12">A744+1</f>
+        <f t="shared" si="11"/>
         <v>745</v>
       </c>
       <c r="B745" s="4" t="s">
@@ -37923,7 +37908,7 @@
     </row>
     <row r="746" spans="1:6">
       <c r="A746">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>746</v>
       </c>
       <c r="B746" s="4" t="s">
@@ -37944,7 +37929,7 @@
     </row>
     <row r="747" spans="1:6">
       <c r="A747">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>747</v>
       </c>
       <c r="B747" s="4" t="s">
@@ -37965,7 +37950,7 @@
     </row>
     <row r="748" spans="1:6">
       <c r="A748">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>748</v>
       </c>
       <c r="B748" s="4" t="s">
@@ -37986,7 +37971,7 @@
     </row>
     <row r="749" spans="1:6">
       <c r="A749">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>749</v>
       </c>
       <c r="B749" s="4" t="s">
@@ -38007,7 +37992,7 @@
     </row>
     <row r="750" spans="1:6">
       <c r="A750">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>750</v>
       </c>
       <c r="B750" s="4" t="s">
@@ -38028,7 +38013,7 @@
     </row>
     <row r="751" spans="1:6">
       <c r="A751">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>751</v>
       </c>
       <c r="B751" s="4" t="s">
@@ -38049,7 +38034,7 @@
     </row>
     <row r="752" spans="1:6">
       <c r="A752">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>752</v>
       </c>
       <c r="B752" s="4" t="s">
@@ -38070,7 +38055,7 @@
     </row>
     <row r="753" spans="1:6">
       <c r="A753">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>753</v>
       </c>
       <c r="B753" s="4" t="s">
@@ -38091,7 +38076,7 @@
     </row>
     <row r="754" spans="1:6">
       <c r="A754">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>754</v>
       </c>
       <c r="B754" s="4" t="s">
@@ -38112,7 +38097,7 @@
     </row>
     <row r="755" spans="1:6">
       <c r="A755">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>755</v>
       </c>
       <c r="B755" s="4" t="s">
@@ -38133,7 +38118,7 @@
     </row>
     <row r="756" spans="1:6">
       <c r="A756">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>756</v>
       </c>
       <c r="B756" s="4" t="s">
@@ -38154,7 +38139,7 @@
     </row>
     <row r="757" spans="1:6">
       <c r="A757">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>757</v>
       </c>
       <c r="B757" s="4" t="s">
@@ -38175,7 +38160,7 @@
     </row>
     <row r="758" spans="1:6">
       <c r="A758">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>758</v>
       </c>
       <c r="B758" s="4" t="s">
@@ -38196,7 +38181,7 @@
     </row>
     <row r="759" spans="1:6">
       <c r="A759">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>759</v>
       </c>
       <c r="B759" s="4" t="s">
@@ -38217,7 +38202,7 @@
     </row>
     <row r="760" spans="1:6">
       <c r="A760">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>760</v>
       </c>
       <c r="B760" s="4" t="s">
@@ -38238,7 +38223,7 @@
     </row>
     <row r="761" spans="1:6">
       <c r="A761">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>761</v>
       </c>
       <c r="B761" s="4" t="s">
@@ -38259,7 +38244,7 @@
     </row>
     <row r="762" spans="1:6">
       <c r="A762">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>762</v>
       </c>
       <c r="B762" s="4" t="s">
@@ -38280,7 +38265,7 @@
     </row>
     <row r="763" spans="1:6">
       <c r="A763">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>763</v>
       </c>
       <c r="B763" s="4" t="s">
@@ -38301,7 +38286,7 @@
     </row>
     <row r="764" spans="1:6">
       <c r="A764">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>764</v>
       </c>
       <c r="B764" s="4" t="s">
@@ -38322,7 +38307,7 @@
     </row>
     <row r="765" spans="1:6">
       <c r="A765">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>765</v>
       </c>
       <c r="B765" s="4" t="s">
@@ -38343,7 +38328,7 @@
     </row>
     <row r="766" spans="1:6">
       <c r="A766">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>766</v>
       </c>
       <c r="B766" s="4" t="s">
@@ -38364,7 +38349,7 @@
     </row>
     <row r="767" spans="1:6">
       <c r="A767">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>767</v>
       </c>
       <c r="B767" s="4" t="s">
@@ -38385,7 +38370,7 @@
     </row>
     <row r="768" spans="1:6">
       <c r="A768">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>768</v>
       </c>
       <c r="B768" s="4" t="s">
@@ -38406,7 +38391,7 @@
     </row>
     <row r="769" spans="1:6">
       <c r="A769">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>769</v>
       </c>
       <c r="B769" s="4" t="s">
@@ -38427,7 +38412,7 @@
     </row>
     <row r="770" spans="1:6">
       <c r="A770">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>770</v>
       </c>
       <c r="B770" s="4" t="s">
@@ -38448,7 +38433,7 @@
     </row>
     <row r="771" spans="1:6">
       <c r="A771">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="A771:A803" si="12">A770+1</f>
         <v>771</v>
       </c>
       <c r="B771" s="4" t="s">

</xml_diff>